<commit_message>
Added logic for multi browser test execution_1
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\Kaman_ECTEST_IE_Support\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2924AE-D4AD-42A4-B827-2AE2DC59A7C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949B9900-78C2-4F9A-8101-1A7310F39E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="72">
   <si>
     <t>Runmode</t>
   </si>
@@ -257,12 +257,6 @@
   </si>
   <si>
     <t>TC23_Verify_UserRegistration</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Yes</t>
@@ -919,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -966,7 +960,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -986,7 +980,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -1006,7 +1000,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -1026,7 +1020,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -1046,7 +1040,7 @@
         <v>59</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
@@ -1066,7 +1060,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
@@ -1086,7 +1080,7 @@
         <v>28</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
@@ -1106,7 +1100,7 @@
         <v>26</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
@@ -1126,7 +1120,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
@@ -1146,7 +1140,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
@@ -1166,7 +1160,7 @@
         <v>36</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
@@ -1186,7 +1180,7 @@
         <v>48</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
@@ -1206,7 +1200,7 @@
         <v>38</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>10</v>
@@ -1226,7 +1220,7 @@
         <v>40</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>10</v>
@@ -1246,7 +1240,7 @@
         <v>42</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>10</v>
@@ -1266,7 +1260,7 @@
         <v>43</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>10</v>
@@ -1286,7 +1280,7 @@
         <v>43</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>10</v>
@@ -1306,7 +1300,7 @@
         <v>46</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>10</v>
@@ -1326,7 +1320,7 @@
         <v>51</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>10</v>
@@ -1346,7 +1340,7 @@
         <v>55</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>10</v>
@@ -1366,7 +1360,7 @@
         <v>57</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>10</v>
@@ -1386,7 +1380,7 @@
         <v>64</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>10</v>
@@ -1406,7 +1400,7 @@
         <v>65</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>10</v>
@@ -1426,7 +1420,7 @@
         <v>69</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>10</v>
@@ -1446,7 +1440,7 @@
         <v>57</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>10</v>
@@ -1466,7 +1460,7 @@
         <v>23</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>10</v>
@@ -1486,7 +1480,7 @@
         <v>61</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>10</v>
@@ -1506,7 +1500,7 @@
         <v>21</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>10</v>
@@ -1526,7 +1520,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>10</v>
@@ -1546,7 +1540,7 @@
         <v>20</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>10</v>
@@ -1566,7 +1560,7 @@
         <v>18</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Ädding FF files , New logic for Email generation, New logic for Full page screenshots
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\Kaman_ECTEST_IE_Support\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949B9900-78C2-4F9A-8101-1A7310F39E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BEC183-EFB8-46CA-9B9F-FB85AE3A909D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,7 +398,107 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{A444948E-6AA8-45F3-AB40-38513383CF85}"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -914,7 +1014,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E2" sqref="E2:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1588,54 +1688,84 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F21:F32">
-    <cfRule type="uniqueValues" dxfId="16" priority="613"/>
+    <cfRule type="uniqueValues" dxfId="26" priority="623"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E33">
-    <cfRule type="uniqueValues" dxfId="15" priority="74"/>
+    <cfRule type="uniqueValues" dxfId="25" priority="84"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E33">
-    <cfRule type="uniqueValues" dxfId="14" priority="29"/>
+    <cfRule type="uniqueValues" dxfId="24" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E33">
-    <cfRule type="uniqueValues" dxfId="13" priority="614"/>
+    <cfRule type="uniqueValues" dxfId="23" priority="624"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E27">
-    <cfRule type="uniqueValues" dxfId="12" priority="25"/>
+    <cfRule type="uniqueValues" dxfId="22" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E33">
-    <cfRule type="uniqueValues" dxfId="11" priority="22"/>
+    <cfRule type="uniqueValues" dxfId="21" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="uniqueValues" dxfId="10" priority="17"/>
+    <cfRule type="uniqueValues" dxfId="20" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="uniqueValues" dxfId="19" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="uniqueValues" dxfId="18" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="uniqueValues" dxfId="17" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="uniqueValues" dxfId="16" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="uniqueValues" dxfId="15" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="uniqueValues" dxfId="14" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="uniqueValues" dxfId="13" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E33">
+    <cfRule type="uniqueValues" dxfId="12" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="uniqueValues" dxfId="11" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E33">
+    <cfRule type="uniqueValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E33">
     <cfRule type="uniqueValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="E2:E33">
     <cfRule type="uniqueValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+  <conditionalFormatting sqref="E2:E33">
     <cfRule type="uniqueValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E23:E33">
     <cfRule type="uniqueValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E33">
+  <conditionalFormatting sqref="E4">
     <cfRule type="uniqueValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E33">
+  <conditionalFormatting sqref="E4">
     <cfRule type="uniqueValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E33">
+  <conditionalFormatting sqref="E4">
     <cfRule type="uniqueValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E33">
+  <conditionalFormatting sqref="E9">
     <cfRule type="uniqueValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E33">
+  <conditionalFormatting sqref="E9">
     <cfRule type="uniqueValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E33">
+  <conditionalFormatting sqref="E9">
     <cfRule type="uniqueValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enabling all testcases ECTEST
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A899F5-F096-449B-9DC7-07D068D42ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537F132F-2BCA-4AAD-8DAF-CF93F941FB40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="72">
   <si>
     <t>Runmode</t>
   </si>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1976,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:E33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2023,7 +2020,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -2043,7 +2040,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -2063,7 +2060,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -2083,7 +2080,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -2103,7 +2100,7 @@
         <v>59</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
@@ -2123,7 +2120,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
@@ -2143,7 +2140,7 @@
         <v>28</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
@@ -2163,7 +2160,7 @@
         <v>26</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
@@ -2183,7 +2180,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
@@ -2203,7 +2200,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
@@ -2223,7 +2220,7 @@
         <v>36</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
@@ -2243,7 +2240,7 @@
         <v>48</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
@@ -2263,7 +2260,7 @@
         <v>38</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>10</v>
@@ -2283,7 +2280,7 @@
         <v>40</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>10</v>
@@ -2303,7 +2300,7 @@
         <v>42</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>10</v>
@@ -2323,7 +2320,7 @@
         <v>43</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>10</v>
@@ -2343,7 +2340,7 @@
         <v>43</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>10</v>
@@ -2363,7 +2360,7 @@
         <v>46</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>10</v>
@@ -2383,7 +2380,7 @@
         <v>51</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>10</v>
@@ -2403,7 +2400,7 @@
         <v>55</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>10</v>
@@ -2423,7 +2420,7 @@
         <v>57</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>10</v>
@@ -2443,7 +2440,7 @@
         <v>64</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>10</v>
@@ -2463,7 +2460,7 @@
         <v>65</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>10</v>
@@ -2503,7 +2500,7 @@
         <v>57</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>10</v>
@@ -2523,7 +2520,7 @@
         <v>23</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>10</v>
@@ -2543,7 +2540,7 @@
         <v>61</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>10</v>
@@ -2563,7 +2560,7 @@
         <v>21</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>10</v>
@@ -2583,7 +2580,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>10</v>
@@ -2603,7 +2600,7 @@
         <v>20</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>10</v>
@@ -2623,7 +2620,7 @@
         <v>18</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>10</v>
@@ -2643,7 +2640,7 @@
         <v>67</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Removed Testase [9:41 AM] Archana Mithoor
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49225812-82C7-4E35-8697-7DAD5DDCCCB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D016AC6-8AF2-409D-9E25-84D37159B010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="MasterExecutor" sheetId="10" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MasterExecutor!$A$1:$F$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MasterExecutor!$A$1:$F$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="71">
   <si>
     <t>Runmode</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Verify Behaviour for PunchOut User</t>
   </si>
   <si>
-    <t>TC24_Verify_PlaceOrder_LoggedIn</t>
-  </si>
-  <si>
     <t>TC02_Verify_MYACC_RegisteredUser</t>
   </si>
   <si>
@@ -395,87 +392,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{A444948E-6AA8-45F3-AB40-38513383CF85}"/>
   </cellStyles>
-  <dxfs count="522">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="514">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5958,10 +5875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6007,7 +5924,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -6027,7 +5944,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -6047,7 +5964,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -6067,7 +5984,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -6087,7 +6004,7 @@
         <v>59</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
@@ -6107,7 +6024,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
@@ -6127,7 +6044,7 @@
         <v>28</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
@@ -6147,7 +6064,7 @@
         <v>26</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
@@ -6167,7 +6084,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
@@ -6187,7 +6104,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
@@ -6207,7 +6124,7 @@
         <v>36</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
@@ -6227,7 +6144,7 @@
         <v>48</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
@@ -6247,7 +6164,7 @@
         <v>38</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>10</v>
@@ -6267,7 +6184,7 @@
         <v>40</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>10</v>
@@ -6287,7 +6204,7 @@
         <v>42</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>10</v>
@@ -6307,7 +6224,7 @@
         <v>43</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>10</v>
@@ -6327,7 +6244,7 @@
         <v>43</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>10</v>
@@ -6347,7 +6264,7 @@
         <v>46</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>10</v>
@@ -6367,7 +6284,7 @@
         <v>51</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>10</v>
@@ -6387,7 +6304,7 @@
         <v>55</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>10</v>
@@ -6407,7 +6324,7 @@
         <v>57</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>10</v>
@@ -6421,13 +6338,13 @@
         <v>7</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>10</v>
@@ -6441,13 +6358,13 @@
         <v>7</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>10</v>
@@ -6461,33 +6378,33 @@
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>71</v>
-      </c>
       <c r="E25" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>10</v>
@@ -6501,13 +6418,13 @@
         <v>7</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>10</v>
@@ -6520,14 +6437,14 @@
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>60</v>
+      <c r="C28" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>10</v>
@@ -6541,13 +6458,13 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>21</v>
+        <v>52</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>10</v>
@@ -6561,39 +6478,39 @@
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="7" t="s">
+    <row r="31" spans="1:6" ht="45">
+      <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="45">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
@@ -6601,1604 +6518,1560 @@
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30">
-      <c r="A33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F33" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E33">
-    <cfRule type="uniqueValues" dxfId="521" priority="719"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="520" priority="674"/>
+    <cfRule type="uniqueValues" dxfId="513" priority="674"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="519" priority="1259"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23:E24 E26:E33">
-    <cfRule type="uniqueValues" dxfId="518" priority="670"/>
+    <cfRule type="uniqueValues" dxfId="512" priority="1259"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="517" priority="667"/>
+    <cfRule type="uniqueValues" dxfId="511" priority="667"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="uniqueValues" dxfId="516" priority="662"/>
+    <cfRule type="uniqueValues" dxfId="510" priority="662"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="515" priority="655"/>
+    <cfRule type="uniqueValues" dxfId="509" priority="655"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="uniqueValues" dxfId="508" priority="654"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="uniqueValues" dxfId="514" priority="654"/>
+    <cfRule type="uniqueValues" dxfId="507" priority="653"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="uniqueValues" dxfId="513" priority="653"/>
+    <cfRule type="uniqueValues" dxfId="506" priority="652"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="505" priority="651"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="504" priority="650"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="503" priority="649"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="502" priority="648"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="501" priority="647"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="500" priority="646"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="499" priority="645"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="498" priority="644"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="497" priority="643"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:E24">
+    <cfRule type="uniqueValues" dxfId="496" priority="642"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="uniqueValues" dxfId="495" priority="641"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="uniqueValues" dxfId="494" priority="640"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="uniqueValues" dxfId="493" priority="639"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="uniqueValues" dxfId="492" priority="638"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="uniqueValues" dxfId="491" priority="637"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="uniqueValues" dxfId="490" priority="636"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:E24">
+    <cfRule type="uniqueValues" dxfId="489" priority="635"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:E31">
+    <cfRule type="uniqueValues" dxfId="488" priority="634"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="uniqueValues" dxfId="512" priority="652"/>
+    <cfRule type="uniqueValues" dxfId="487" priority="633"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="uniqueValues" dxfId="486" priority="632"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="uniqueValues" dxfId="485" priority="631"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="511" priority="651"/>
+    <cfRule type="uniqueValues" dxfId="484" priority="628"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="510" priority="650"/>
+    <cfRule type="uniqueValues" dxfId="483" priority="627"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="509" priority="649"/>
+    <cfRule type="uniqueValues" dxfId="482" priority="626"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="508" priority="648"/>
+    <cfRule type="uniqueValues" dxfId="481" priority="625"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="507" priority="647"/>
+    <cfRule type="uniqueValues" dxfId="480" priority="624"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E5">
+    <cfRule type="uniqueValues" dxfId="479" priority="623"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E5">
+    <cfRule type="uniqueValues" dxfId="478" priority="622"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E5">
+    <cfRule type="uniqueValues" dxfId="477" priority="621"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E5">
+    <cfRule type="uniqueValues" dxfId="476" priority="620"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E5">
+    <cfRule type="uniqueValues" dxfId="475" priority="619"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="506" priority="646"/>
+    <cfRule type="uniqueValues" dxfId="474" priority="618"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="505" priority="645"/>
+    <cfRule type="uniqueValues" dxfId="473" priority="617"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="504" priority="644"/>
+    <cfRule type="uniqueValues" dxfId="472" priority="616"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="503" priority="643"/>
+    <cfRule type="uniqueValues" dxfId="471" priority="615"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="470" priority="614"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="uniqueValues" dxfId="469" priority="613"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="uniqueValues" dxfId="468" priority="610"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="uniqueValues" dxfId="467" priority="608"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="uniqueValues" dxfId="466" priority="607"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="uniqueValues" dxfId="465" priority="605"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="uniqueValues" dxfId="464" priority="604"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="uniqueValues" dxfId="463" priority="603"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="462" priority="602"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="461" priority="601"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="460" priority="600"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="459" priority="599"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="458" priority="598"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E24">
-    <cfRule type="uniqueValues" dxfId="502" priority="642"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="uniqueValues" dxfId="501" priority="641"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="uniqueValues" dxfId="500" priority="640"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="uniqueValues" dxfId="499" priority="639"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
-    <cfRule type="uniqueValues" dxfId="498" priority="638"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
-    <cfRule type="uniqueValues" dxfId="497" priority="637"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
-    <cfRule type="uniqueValues" dxfId="496" priority="636"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23:E24">
-    <cfRule type="uniqueValues" dxfId="495" priority="635"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27:E32">
-    <cfRule type="uniqueValues" dxfId="494" priority="634"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="uniqueValues" dxfId="493" priority="633"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="uniqueValues" dxfId="492" priority="632"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="uniqueValues" dxfId="491" priority="631"/>
+    <cfRule type="uniqueValues" dxfId="457" priority="597"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="456" priority="596"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="455" priority="595"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="454" priority="594"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="453" priority="593"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="uniqueValues" dxfId="452" priority="592"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="uniqueValues" dxfId="490" priority="629"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="489" priority="628"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="488" priority="627"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="487" priority="626"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="486" priority="625"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="485" priority="624"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E5">
-    <cfRule type="uniqueValues" dxfId="484" priority="623"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E5">
-    <cfRule type="uniqueValues" dxfId="483" priority="622"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E5">
-    <cfRule type="uniqueValues" dxfId="482" priority="621"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E5">
-    <cfRule type="uniqueValues" dxfId="481" priority="620"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E5">
-    <cfRule type="uniqueValues" dxfId="480" priority="619"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="479" priority="618"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="478" priority="617"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="477" priority="616"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="476" priority="615"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="475" priority="614"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="uniqueValues" dxfId="474" priority="613"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E33">
-    <cfRule type="uniqueValues" dxfId="473" priority="612"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24 E26:E33">
-    <cfRule type="uniqueValues" dxfId="472" priority="611"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="uniqueValues" dxfId="471" priority="610"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="uniqueValues" dxfId="470" priority="608"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="uniqueValues" dxfId="469" priority="607"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="uniqueValues" dxfId="468" priority="605"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="uniqueValues" dxfId="467" priority="604"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="uniqueValues" dxfId="466" priority="603"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="465" priority="602"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="464" priority="601"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="463" priority="600"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="462" priority="599"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="461" priority="598"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23:E24">
-    <cfRule type="uniqueValues" dxfId="460" priority="597"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="459" priority="596"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="458" priority="595"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="457" priority="594"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="456" priority="593"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E21">
-    <cfRule type="uniqueValues" dxfId="455" priority="592"/>
+    <cfRule type="uniqueValues" dxfId="451" priority="587"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="uniqueValues" dxfId="454" priority="591"/>
+    <cfRule type="uniqueValues" dxfId="450" priority="586"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="uniqueValues" dxfId="453" priority="590"/>
+    <cfRule type="uniqueValues" dxfId="449" priority="585"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="uniqueValues" dxfId="452" priority="589"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="uniqueValues" dxfId="451" priority="587"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="uniqueValues" dxfId="450" priority="586"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="uniqueValues" dxfId="449" priority="585"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
     <cfRule type="uniqueValues" dxfId="448" priority="584"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
-    <cfRule type="uniqueValues" dxfId="447" priority="583"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
-    <cfRule type="uniqueValues" dxfId="446" priority="582"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
-    <cfRule type="uniqueValues" dxfId="445" priority="581"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
-    <cfRule type="uniqueValues" dxfId="444" priority="580"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="443" priority="579"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="442" priority="578"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="441" priority="577"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="440" priority="576"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="439" priority="575"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="438" priority="574"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="437" priority="573"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="436" priority="572"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="uniqueValues" dxfId="435" priority="571"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="uniqueValues" dxfId="434" priority="570"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="uniqueValues" dxfId="433" priority="569"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="uniqueValues" dxfId="432" priority="568"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="uniqueValues" dxfId="431" priority="567"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="uniqueValues" dxfId="430" priority="566"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="uniqueValues" dxfId="429" priority="565"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="uniqueValues" dxfId="428" priority="564"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="427" priority="563"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="426" priority="562"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="425" priority="561"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="424" priority="560"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="423" priority="559"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="422" priority="558"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="421" priority="557"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="420" priority="556"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="419" priority="555"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="418" priority="554"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="417" priority="553"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="416" priority="552"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="415" priority="551"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="414" priority="550"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="413" priority="549"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="uniqueValues" dxfId="412" priority="548"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="411" priority="547"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="410" priority="546"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="409" priority="545"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="408" priority="544"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="407" priority="543"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="406" priority="542"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="405" priority="541"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33">
-    <cfRule type="uniqueValues" dxfId="404" priority="540"/>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="447" priority="579"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="446" priority="578"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="445" priority="577"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="444" priority="576"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="443" priority="575"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="442" priority="574"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="441" priority="573"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="440" priority="572"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="uniqueValues" dxfId="439" priority="571"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="uniqueValues" dxfId="438" priority="570"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="uniqueValues" dxfId="437" priority="569"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="uniqueValues" dxfId="436" priority="568"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="uniqueValues" dxfId="435" priority="567"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="uniqueValues" dxfId="434" priority="566"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="uniqueValues" dxfId="433" priority="565"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="uniqueValues" dxfId="432" priority="564"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="431" priority="563"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="430" priority="562"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="429" priority="561"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="428" priority="560"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="427" priority="559"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="426" priority="558"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="425" priority="557"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="424" priority="556"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="423" priority="555"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="422" priority="554"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="421" priority="553"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="420" priority="552"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="419" priority="551"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="418" priority="550"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="417" priority="549"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="uniqueValues" dxfId="416" priority="548"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="415" priority="547"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="414" priority="546"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="413" priority="545"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="412" priority="544"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="411" priority="543"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="410" priority="542"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="409" priority="541"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="uniqueValues" dxfId="408" priority="540"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="403" priority="402"/>
+    <cfRule type="uniqueValues" dxfId="407" priority="402"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="402" priority="401"/>
+    <cfRule type="uniqueValues" dxfId="406" priority="401"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="401" priority="403"/>
+    <cfRule type="uniqueValues" dxfId="405" priority="403"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="400" priority="400"/>
+    <cfRule type="uniqueValues" dxfId="404" priority="400"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="399" priority="399"/>
+    <cfRule type="uniqueValues" dxfId="403" priority="399"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="398" priority="398"/>
+    <cfRule type="uniqueValues" dxfId="402" priority="398"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="397" priority="397"/>
+    <cfRule type="uniqueValues" dxfId="401" priority="397"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="396" priority="396"/>
+    <cfRule type="uniqueValues" dxfId="400" priority="396"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="395" priority="395"/>
+    <cfRule type="uniqueValues" dxfId="399" priority="395"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="394" priority="394"/>
+    <cfRule type="uniqueValues" dxfId="398" priority="394"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="393" priority="393"/>
+    <cfRule type="uniqueValues" dxfId="397" priority="393"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="392" priority="392"/>
+    <cfRule type="uniqueValues" dxfId="396" priority="392"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="391" priority="391"/>
+    <cfRule type="uniqueValues" dxfId="395" priority="391"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="390" priority="390"/>
+    <cfRule type="uniqueValues" dxfId="394" priority="390"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="389" priority="389"/>
+    <cfRule type="uniqueValues" dxfId="393" priority="389"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="388" priority="388"/>
+    <cfRule type="uniqueValues" dxfId="392" priority="388"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="387" priority="387"/>
+    <cfRule type="uniqueValues" dxfId="391" priority="387"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="386" priority="386"/>
+    <cfRule type="uniqueValues" dxfId="390" priority="386"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="385" priority="385"/>
+    <cfRule type="uniqueValues" dxfId="389" priority="385"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="384" priority="384"/>
+    <cfRule type="uniqueValues" dxfId="388" priority="384"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="383" priority="383"/>
+    <cfRule type="uniqueValues" dxfId="387" priority="383"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="382" priority="382"/>
+    <cfRule type="uniqueValues" dxfId="386" priority="382"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="381" priority="381"/>
+    <cfRule type="uniqueValues" dxfId="385" priority="381"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="380" priority="380"/>
+    <cfRule type="uniqueValues" dxfId="384" priority="380"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="379" priority="379"/>
+    <cfRule type="uniqueValues" dxfId="383" priority="379"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="378" priority="378"/>
+    <cfRule type="uniqueValues" dxfId="382" priority="378"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="377" priority="377"/>
+    <cfRule type="uniqueValues" dxfId="381" priority="377"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="376" priority="376"/>
+    <cfRule type="uniqueValues" dxfId="380" priority="376"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="375" priority="375"/>
+    <cfRule type="uniqueValues" dxfId="379" priority="375"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="374" priority="374"/>
+    <cfRule type="uniqueValues" dxfId="378" priority="374"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="373" priority="373"/>
+    <cfRule type="uniqueValues" dxfId="377" priority="373"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="372" priority="372"/>
+    <cfRule type="uniqueValues" dxfId="376" priority="372"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="371" priority="371"/>
+    <cfRule type="uniqueValues" dxfId="375" priority="371"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="370" priority="370"/>
+    <cfRule type="uniqueValues" dxfId="374" priority="370"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="369" priority="369"/>
+    <cfRule type="uniqueValues" dxfId="373" priority="369"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="368" priority="368"/>
+    <cfRule type="uniqueValues" dxfId="372" priority="368"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="367" priority="367"/>
+    <cfRule type="uniqueValues" dxfId="371" priority="367"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="366" priority="366"/>
+    <cfRule type="uniqueValues" dxfId="370" priority="366"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="365" priority="365"/>
+    <cfRule type="uniqueValues" dxfId="369" priority="365"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="364" priority="364"/>
+    <cfRule type="uniqueValues" dxfId="368" priority="364"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="363" priority="363"/>
+    <cfRule type="uniqueValues" dxfId="367" priority="363"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="362" priority="362"/>
+    <cfRule type="uniqueValues" dxfId="366" priority="362"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="361" priority="361"/>
+    <cfRule type="uniqueValues" dxfId="365" priority="361"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="360" priority="360"/>
+    <cfRule type="uniqueValues" dxfId="364" priority="360"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="uniqueValues" dxfId="359" priority="359"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21:F24 F26:F32">
-    <cfRule type="uniqueValues" dxfId="358" priority="1260"/>
+    <cfRule type="uniqueValues" dxfId="363" priority="359"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="uniqueValues" dxfId="357" priority="358"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="356" priority="355"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="355" priority="354"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="354" priority="353"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="353" priority="352"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="352" priority="351"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="351" priority="350"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="350" priority="349"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="349" priority="348"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="348" priority="347"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="347" priority="346"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="346" priority="345"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="345" priority="344"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="344" priority="343"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="343" priority="342"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="342" priority="341"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="341" priority="340"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="340" priority="339"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="339" priority="338"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="338" priority="337"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="337" priority="336"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="336" priority="335"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="335" priority="334"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="334" priority="333"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="333" priority="332"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="332" priority="331"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="331" priority="330"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="330" priority="329"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="329" priority="328"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="328" priority="327"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="327" priority="326"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="326" priority="356"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="325" priority="357"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="324" priority="325"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="323" priority="324"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="322" priority="323"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="321" priority="322"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="320" priority="321"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="319" priority="320"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="318" priority="319"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="317" priority="318"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="316" priority="317"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="315" priority="316"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="314" priority="314"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="313" priority="313"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="312" priority="312"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="311" priority="311"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="310" priority="310"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="309" priority="309"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="308" priority="308"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="307" priority="307"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="306" priority="306"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="305" priority="305"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="304" priority="304"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="303" priority="303"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="302" priority="302"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="301" priority="301"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="300" priority="300"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="299" priority="315"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="298" priority="298"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="297" priority="297"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="296" priority="296"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="295" priority="295"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="294" priority="294"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="293" priority="293"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="292" priority="292"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="291" priority="291"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="290" priority="290"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="289" priority="289"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="288" priority="288"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="287" priority="287"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="286" priority="286"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="285" priority="285"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="284" priority="284"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="283" priority="299"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="282" priority="283"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="281" priority="282"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="280" priority="281"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="279" priority="280"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="278" priority="279"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="277" priority="278"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="276" priority="277"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="275" priority="276"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="274" priority="275"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="273" priority="274"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="272" priority="273"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="271" priority="272"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="270" priority="271"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="269" priority="270"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="268" priority="269"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="267" priority="268"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="266" priority="267"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="265" priority="266"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="264" priority="265"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="263" priority="264"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="262" priority="263"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="261" priority="262"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="260" priority="261"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="259" priority="260"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="258" priority="259"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="257" priority="258"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="256" priority="257"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="255" priority="256"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="254" priority="255"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="253" priority="254"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="252" priority="253"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="251" priority="252"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="250" priority="251"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="249" priority="250"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="248" priority="249"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="247" priority="248"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="246" priority="247"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="245" priority="246"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="244" priority="245"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="243" priority="244"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="242" priority="243"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="241" priority="242"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="240" priority="241"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="239" priority="240"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="238" priority="239"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="237" priority="238"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="236" priority="237"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="235" priority="236"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="234" priority="235"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="233" priority="234"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="232" priority="233"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="231" priority="232"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="230" priority="231"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="229" priority="230"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="228" priority="229"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="227" priority="228"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="226" priority="227"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="225" priority="226"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="224" priority="225"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="223" priority="224"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="222" priority="223"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="221" priority="221"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="220" priority="220"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="219" priority="219"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="218" priority="218"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="217" priority="217"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="216" priority="216"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="215" priority="215"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="214" priority="214"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="213" priority="213"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="212" priority="212"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="211" priority="211"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="210" priority="210"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="209" priority="209"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="208" priority="208"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="207" priority="207"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="206" priority="222"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="205" priority="206"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="204" priority="205"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="203" priority="204"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="202" priority="203"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="201" priority="202"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="200" priority="201"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="199" priority="200"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="198" priority="199"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="197" priority="198"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="196" priority="197"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="195" priority="196"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="194" priority="195"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="193" priority="194"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="192" priority="193"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="191" priority="192"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="190" priority="191"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="189" priority="189"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="188" priority="188"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="187" priority="187"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="186" priority="186"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="185" priority="185"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="184" priority="184"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="183" priority="183"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="182" priority="182"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="181" priority="181"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="180" priority="180"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="179" priority="179"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="178" priority="178"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="177" priority="177"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="176" priority="176"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="175" priority="175"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="174" priority="190"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="173" priority="174"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="172" priority="173"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="171" priority="172"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="170" priority="171"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="169" priority="170"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="168" priority="169"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="167" priority="168"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="166" priority="167"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="165" priority="166"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="164" priority="165"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="163" priority="164"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="162" priority="163"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="161" priority="162"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="160" priority="161"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="159" priority="160"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="158" priority="159"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="157" priority="158"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="156" priority="157"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="155" priority="156"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="154" priority="155"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="153" priority="154"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="152" priority="153"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="151" priority="152"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="150" priority="151"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="149" priority="150"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="148" priority="149"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="147" priority="148"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="146" priority="147"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="145" priority="146"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="144" priority="145"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="143" priority="144"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="142" priority="143"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="141" priority="142"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="140" priority="141"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="139" priority="140"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="138" priority="139"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="137" priority="138"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="136" priority="137"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="135" priority="136"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="134" priority="135"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="133" priority="134"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="132" priority="133"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="131" priority="132"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="130" priority="131"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="129" priority="130"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="128" priority="129"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="127" priority="128"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="126" priority="127"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="125" priority="126"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="124" priority="125"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="123" priority="124"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="122" priority="123"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="121" priority="122"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="120" priority="121"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="119" priority="120"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="118" priority="119"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="117" priority="118"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="116" priority="117"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="115" priority="116"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="114" priority="115"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="113" priority="114"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="112" priority="113"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="111" priority="112"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="110" priority="111"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="109" priority="110"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="108" priority="109"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="107" priority="107"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="106" priority="106"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="105" priority="105"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="104" priority="104"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="103" priority="103"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="102" priority="102"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="101" priority="101"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="100" priority="100"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="99" priority="99"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="98" priority="98"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="97" priority="97"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="96" priority="96"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="95" priority="95"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="94" priority="94"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="93" priority="93"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="92" priority="108"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="91" priority="92"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="90" priority="91"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="89" priority="90"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="88" priority="89"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="87" priority="88"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="86" priority="87"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="85" priority="86"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="84" priority="85"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="83" priority="84"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="82" priority="83"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="81" priority="82"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="80" priority="81"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="79" priority="80"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="78" priority="79"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="77" priority="78"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="76" priority="77"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="75" priority="76"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="74" priority="75"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="73" priority="74"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="72" priority="73"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="71" priority="72"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="70" priority="71"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="69" priority="70"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="68" priority="69"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="67" priority="68"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="66" priority="67"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="65" priority="66"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="64" priority="65"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="63" priority="64"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="62" priority="63"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="61" priority="62"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="60" priority="61"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="59" priority="60"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="58" priority="59"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="57" priority="58"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="56" priority="57"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="55" priority="56"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="54" priority="55"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="53" priority="54"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="52" priority="53"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="51" priority="52"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="50" priority="51"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="49" priority="50"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="48" priority="49"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="47" priority="48"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="46" priority="47"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="45" priority="46"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="44" priority="45"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="43" priority="44"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="42" priority="43"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="41" priority="42"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="40" priority="41"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="39" priority="40"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="38" priority="39"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="37" priority="38"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="36" priority="37"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="35" priority="36"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="34" priority="35"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="33" priority="34"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="32" priority="33"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="31" priority="31"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="30" priority="30"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="29" priority="29"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="28" priority="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="27" priority="27"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="26" priority="26"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="25" priority="25"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="24" priority="24"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="23" priority="23"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="22" priority="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="21" priority="21"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="20" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="19" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="18" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="17" priority="17"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="16" priority="32"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="15" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="14" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="13" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="12" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="11" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="10" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="9" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="8" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="7" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="6" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="5" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="4" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
+    <cfRule type="uniqueValues" dxfId="362" priority="358"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="361" priority="355"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="360" priority="354"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="359" priority="353"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="358" priority="352"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="357" priority="351"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="356" priority="350"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="355" priority="349"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="354" priority="348"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="353" priority="347"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="352" priority="346"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="351" priority="345"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="350" priority="344"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="349" priority="343"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="348" priority="342"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="347" priority="341"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="346" priority="340"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="345" priority="339"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="344" priority="338"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="343" priority="337"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="342" priority="336"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="341" priority="335"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="340" priority="334"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="339" priority="333"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="338" priority="332"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="337" priority="331"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="336" priority="330"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="335" priority="329"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="334" priority="328"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="333" priority="327"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="332" priority="326"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="331" priority="356"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="330" priority="357"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="329" priority="325"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="328" priority="324"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="327" priority="323"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="326" priority="322"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="325" priority="321"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="324" priority="320"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="323" priority="319"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="322" priority="318"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="321" priority="317"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="320" priority="316"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="319" priority="314"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="318" priority="313"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="317" priority="312"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="316" priority="311"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="315" priority="310"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="314" priority="309"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="313" priority="308"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="312" priority="307"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="311" priority="306"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="310" priority="305"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="309" priority="304"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="308" priority="303"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="307" priority="302"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="306" priority="301"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="305" priority="300"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="304" priority="315"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="303" priority="298"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="302" priority="297"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="301" priority="296"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="300" priority="295"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="299" priority="294"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="298" priority="293"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="297" priority="292"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="296" priority="291"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="295" priority="290"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="294" priority="289"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="293" priority="288"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="292" priority="287"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="291" priority="286"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="290" priority="285"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="289" priority="284"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="288" priority="299"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="287" priority="283"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="286" priority="282"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="285" priority="281"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="284" priority="280"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="283" priority="279"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="282" priority="278"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="281" priority="277"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="280" priority="276"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="279" priority="275"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="278" priority="274"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="277" priority="273"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="276" priority="272"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="275" priority="271"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="274" priority="270"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="273" priority="269"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="272" priority="268"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="271" priority="267"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="270" priority="266"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="269" priority="265"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="268" priority="264"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="267" priority="263"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="266" priority="262"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="265" priority="261"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="264" priority="260"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="263" priority="259"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="262" priority="258"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="261" priority="257"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="260" priority="256"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="259" priority="255"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="258" priority="254"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="257" priority="253"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="256" priority="252"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="255" priority="251"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="254" priority="250"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="253" priority="249"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="252" priority="248"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="251" priority="247"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="250" priority="246"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="249" priority="245"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="248" priority="244"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="247" priority="243"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="246" priority="242"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="245" priority="241"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="244" priority="240"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="243" priority="239"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="242" priority="238"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="241" priority="237"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="240" priority="236"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="239" priority="235"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="238" priority="234"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="237" priority="233"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="236" priority="232"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="235" priority="231"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="234" priority="230"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="233" priority="229"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="232" priority="228"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="231" priority="227"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="230" priority="226"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="229" priority="225"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="228" priority="224"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="227" priority="223"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="226" priority="221"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="225" priority="220"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="224" priority="219"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="223" priority="218"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="222" priority="217"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="221" priority="216"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="220" priority="215"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="219" priority="214"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="218" priority="213"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="217" priority="212"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="216" priority="211"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="215" priority="210"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="214" priority="209"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="213" priority="208"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="212" priority="207"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="211" priority="222"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="210" priority="206"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="209" priority="205"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="208" priority="204"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="207" priority="203"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="206" priority="202"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="205" priority="201"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="204" priority="200"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="203" priority="199"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="202" priority="198"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="201" priority="197"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="200" priority="196"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="199" priority="195"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="198" priority="194"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="197" priority="193"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="196" priority="192"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="195" priority="191"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="194" priority="189"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="193" priority="188"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="192" priority="187"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="191" priority="186"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="190" priority="185"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="189" priority="184"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="188" priority="183"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="187" priority="182"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="186" priority="181"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="185" priority="180"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="184" priority="179"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="183" priority="178"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="182" priority="177"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="181" priority="176"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="180" priority="175"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="179" priority="190"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="178" priority="174"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="177" priority="173"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="176" priority="172"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="175" priority="171"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="174" priority="170"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="173" priority="169"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="172" priority="168"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="171" priority="167"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="170" priority="166"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="169" priority="165"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="168" priority="164"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="167" priority="163"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="166" priority="162"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="165" priority="161"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="164" priority="160"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="163" priority="159"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="162" priority="158"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="161" priority="157"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="160" priority="156"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="159" priority="155"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="158" priority="154"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="157" priority="153"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="156" priority="152"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="155" priority="151"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="154" priority="150"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="153" priority="149"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="152" priority="148"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="151" priority="147"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="150" priority="146"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="149" priority="145"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="148" priority="144"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="147" priority="143"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="146" priority="142"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="145" priority="141"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="144" priority="140"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="143" priority="139"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="142" priority="138"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="141" priority="137"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="140" priority="136"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="139" priority="135"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="138" priority="134"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="137" priority="133"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="136" priority="132"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="135" priority="131"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="134" priority="130"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="133" priority="129"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="132" priority="128"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="131" priority="127"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="130" priority="126"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="129" priority="125"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="128" priority="124"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="127" priority="123"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="126" priority="122"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="125" priority="121"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="124" priority="120"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="123" priority="119"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="122" priority="118"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="121" priority="117"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="120" priority="116"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="119" priority="115"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="118" priority="114"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="117" priority="113"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="116" priority="112"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="115" priority="111"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="114" priority="110"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="113" priority="109"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="112" priority="107"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="111" priority="106"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="110" priority="105"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="109" priority="104"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="108" priority="103"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="107" priority="102"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="106" priority="101"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="105" priority="100"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="104" priority="99"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="103" priority="98"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="102" priority="97"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="101" priority="96"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="100" priority="95"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="99" priority="94"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="98" priority="93"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="97" priority="108"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="96" priority="92"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="95" priority="91"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="94" priority="90"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="93" priority="89"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="92" priority="88"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="91" priority="87"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="90" priority="86"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="89" priority="85"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="88" priority="84"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="87" priority="83"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="86" priority="82"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="85" priority="81"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="84" priority="80"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="83" priority="79"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="82" priority="78"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="81" priority="77"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="80" priority="76"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="79" priority="75"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="78" priority="74"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="77" priority="73"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="76" priority="72"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="75" priority="71"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="74" priority="70"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="73" priority="69"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="72" priority="68"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="71" priority="67"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="70" priority="66"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="69" priority="65"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="68" priority="64"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="67" priority="63"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="66" priority="62"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="65" priority="61"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="64" priority="60"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="63" priority="59"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="62" priority="58"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="61" priority="57"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="60" priority="56"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="59" priority="55"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="58" priority="54"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="57" priority="53"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="56" priority="52"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="55" priority="51"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="54" priority="50"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="53" priority="49"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="52" priority="48"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="51" priority="47"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="50" priority="46"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="49" priority="45"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="48" priority="44"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="47" priority="43"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="46" priority="42"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="45" priority="41"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="44" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="43" priority="39"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="42" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="41" priority="37"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="40" priority="36"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="39" priority="35"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="38" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="37" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="36" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="35" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="34" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="33" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="32" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="31" priority="26"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="30" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="29" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="28" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="27" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="26" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="25" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="24" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="23" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="22" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="21" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="20" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="19" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="18" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="17" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="16" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="15" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="14" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="13" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="12" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="11" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="10" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="9" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="8" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="7" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="6" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="uniqueValues" dxfId="5" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E32">
+    <cfRule type="uniqueValues" dxfId="4" priority="1261"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:E24 E26:E32">
+    <cfRule type="uniqueValues" dxfId="3" priority="1263"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:E32">
+    <cfRule type="uniqueValues" dxfId="2" priority="1265"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24 E26:E32">
+    <cfRule type="uniqueValues" dxfId="1" priority="1266"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:F24 F26:F31">
+    <cfRule type="uniqueValues" dxfId="0" priority="1268"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed TC24_Verify_PlaceOrder_LoggedIn as functionalilty no longer available
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D34899-5B70-4F4F-AC38-F56C9C42FCCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A9D7B8-5336-44F4-8CCC-EF511CF2608E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5928,7 +5928,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Changed logic for ReadObject_1
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E853B3B7-D170-40C0-9CBA-AACFA814CFCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A1E372-5BB0-420D-B49D-9934E828C777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -747,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes done for Serlf services testcases
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Master_executors\ECTEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC44BF63-C263-4C14-B3E9-08051FC0A19A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6A5D24-B6E4-457F-AE89-F86194049B1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="MasterExecutor" sheetId="10" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MasterExecutor!$A$1:$F$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MasterExecutor!$A$1:$F$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="75">
   <si>
     <t>Runmode</t>
   </si>
@@ -196,9 +196,6 @@
 3.User must be navigated to final check out page</t>
   </si>
   <si>
-    <t>TC22_Verify_PlaceOrder</t>
-  </si>
-  <si>
     <t>Order should be placed successfully</t>
   </si>
   <si>
@@ -255,6 +252,21 @@
   <si>
     <t>1. more than 10 Items should be added to cart
 2. Appropriate inventory message must be displayed</t>
+  </si>
+  <si>
+    <t>TC22_Verify_PlaceOrder_GuestUser</t>
+  </si>
+  <si>
+    <t>TC42_Verify_PlaceOrder_SelfService_SingleUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self Service Single User Should able place order </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self Service Multi User Should able place order </t>
+  </si>
+  <si>
+    <t>TC43_Verify_PlaceOrder_SelfService_MultiUser</t>
   </si>
 </sst>
 </file>
@@ -759,17 +771,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E32"/>
+      <selection activeCell="E2" sqref="E2:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -808,7 +820,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -822,13 +834,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -848,7 +860,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -868,7 +880,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -882,13 +894,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
@@ -908,7 +920,7 @@
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
@@ -928,7 +940,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
@@ -948,7 +960,7 @@
         <v>22</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
@@ -968,7 +980,7 @@
         <v>28</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
@@ -988,7 +1000,7 @@
         <v>30</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
@@ -1008,7 +1020,7 @@
         <v>32</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
@@ -1028,7 +1040,7 @@
         <v>44</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
@@ -1042,13 +1054,13 @@
         <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>65</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>10</v>
@@ -1068,7 +1080,7 @@
         <v>34</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>10</v>
@@ -1088,7 +1100,7 @@
         <v>36</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>10</v>
@@ -1108,7 +1120,7 @@
         <v>38</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>10</v>
@@ -1128,7 +1140,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>10</v>
@@ -1148,7 +1160,7 @@
         <v>39</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>10</v>
@@ -1168,7 +1180,7 @@
         <v>42</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>10</v>
@@ -1188,7 +1200,7 @@
         <v>47</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>10</v>
@@ -1208,7 +1220,7 @@
         <v>51</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>10</v>
@@ -1222,37 +1234,27 @@
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>53</v>
-      </c>
       <c r="E23" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>10</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
@@ -1262,13 +1264,13 @@
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E25" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>10</v>
@@ -1282,33 +1284,33 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>19</v>
-      </c>
       <c r="E27" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>10</v>
@@ -1322,13 +1324,13 @@
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>10</v>
@@ -1342,13 +1344,13 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>10</v>
@@ -1362,13 +1364,13 @@
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>49</v>
+        <v>18</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>10</v>
@@ -1382,43 +1384,103 @@
         <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30">
-      <c r="A32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="E32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30">
+      <c r="A33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="E33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F26">
+  <conditionalFormatting sqref="F27">
     <cfRule type="uniqueValues" dxfId="1" priority="3702"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F25 F27:F31">
+  <conditionalFormatting sqref="F22:F26 F28:F32">
     <cfRule type="uniqueValues" dxfId="0" priority="4613"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix for TC22 File name
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6A5D24-B6E4-457F-AE89-F86194049B1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC34532-318E-4EE6-B3D7-3D0089FFBE68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="MasterExecutor" sheetId="10" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MasterExecutor!$A$1:$F$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MasterExecutor!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="75">
   <si>
     <t>Runmode</t>
   </si>
@@ -273,7 +273,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -304,12 +304,6 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -377,7 +371,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -402,7 +396,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E35"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -833,7 +826,7 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -1233,7 +1226,7 @@
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="5" t="s">
         <v>70</v>
       </c>
       <c r="D23" s="10" t="s">
@@ -1247,14 +1240,24 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="10"/>
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="E24" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
@@ -1264,10 +1267,10 @@
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>65</v>
@@ -1284,10 +1287,10 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>65</v>
@@ -1297,17 +1300,17 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>65</v>
@@ -1324,10 +1327,10 @@
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>65</v>
@@ -1344,10 +1347,10 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>65</v>
@@ -1364,10 +1367,10 @@
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>17</v>
+        <v>48</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>65</v>
@@ -1384,10 +1387,10 @@
         <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>49</v>
+        <v>15</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>65</v>
@@ -1396,27 +1399,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:6" ht="30">
+      <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30">
+      <c r="F32" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
@@ -1424,10 +1427,10 @@
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>65</v>
@@ -1443,11 +1446,11 @@
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>71</v>
+      <c r="C34" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>65</v>
@@ -1456,31 +1459,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="F27">
+  <conditionalFormatting sqref="F26">
     <cfRule type="uniqueValues" dxfId="1" priority="3702"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F26 F28:F32">
+  <conditionalFormatting sqref="F27:F31 F22:F25">
     <cfRule type="uniqueValues" dxfId="0" priority="4613"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
enabling punchout testcase for ECTEST
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F8220D-A8F7-4AAA-8095-90FD5E700809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB6AFC8-88DA-429E-8B02-3CE26C61346C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="75">
   <si>
     <t>Runmode</t>
   </si>
@@ -231,9 +231,6 @@
     <t xml:space="preserve">Verifying Product comparison </t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>TC03_Verify_BLP_Solutions_ContactUS</t>
   </si>
   <si>
@@ -261,6 +258,15 @@
   </si>
   <si>
     <t>TC43_Verify_PlaceOrder_SelfService_MultiUser</t>
+  </si>
+  <si>
+    <t>Order should be placed successfully using Punchout user</t>
+  </si>
+  <si>
+    <t>TC28_Verify_PunchOut_User</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -758,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -801,33 +807,33 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>70</v>
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="D3" s="10" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -841,19 +847,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -861,19 +867,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>65</v>
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="45">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -881,13 +887,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
+        <v>53</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
@@ -901,19 +907,19 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -921,13 +927,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>54</v>
+        <v>23</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
@@ -941,13 +947,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
@@ -961,13 +967,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
@@ -981,113 +987,113 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>22</v>
+        <v>29</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>28</v>
+      <c r="C12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>29</v>
+      <c r="C13" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>31</v>
+      <c r="C14" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:6" ht="30">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>43</v>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>62</v>
+      <c r="C16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>10</v>
@@ -1100,16 +1106,16 @@
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
+      <c r="C17" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1120,34 +1126,34 @@
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>36</v>
+      <c r="C18" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>38</v>
+      <c r="C19" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>10</v>
@@ -1160,14 +1166,14 @@
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>39</v>
+      <c r="C20" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>10</v>
@@ -1180,36 +1186,36 @@
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>39</v>
+      <c r="C21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="45">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>41</v>
+      <c r="C22" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1220,20 +1226,20 @@
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>46</v>
+      <c r="C23" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45">
+        <v>74</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -1241,13 +1247,13 @@
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>51</v>
+        <v>58</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>10</v>
@@ -1260,14 +1266,14 @@
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>52</v>
+      <c r="C25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>10</v>
@@ -1281,53 +1287,53 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>57</v>
+        <v>20</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>10</v>
@@ -1341,13 +1347,13 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>10</v>
@@ -1361,13 +1367,13 @@
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>17</v>
+        <v>48</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>10</v>
@@ -1381,39 +1387,39 @@
         <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>49</v>
+        <v>15</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:6" ht="30">
+      <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30">
+        <v>74</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
@@ -1421,23 +1427,43 @@
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F28">
+  <conditionalFormatting sqref="F26">
     <cfRule type="uniqueValues" dxfId="1" priority="3702"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29:F32 F24:F27">
+  <conditionalFormatting sqref="F22:F25 F27:F31">
     <cfRule type="uniqueValues" dxfId="0" priority="4614"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ECTEST TC25 & TC32 Disabled
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68D6D52-8931-44BA-A7E4-2BA7FA5B300E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CC5607-D517-41BD-931C-679ACA036F8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="72">
   <si>
     <t>Runmode</t>
   </si>
@@ -198,12 +198,6 @@
     <t>Verify PDP Page</t>
   </si>
   <si>
-    <t>TC25_Verify_Footer</t>
-  </si>
-  <si>
-    <t>Verify  all Footer content</t>
-  </si>
-  <si>
     <t>TC26_Adding_MultipleItems_QuickOrder</t>
   </si>
   <si>
@@ -243,13 +237,7 @@
     <t>User should able to add mutiple items and place order</t>
   </si>
   <si>
-    <t>TC32_Verify_PlaceOrder_ManagedUser</t>
-  </si>
-  <si>
     <t>TC33_Price_Verification_on_CartPage</t>
-  </si>
-  <si>
-    <t>Managed User should able to place order</t>
   </si>
   <si>
     <t>price for listed items should be dispalyed</t>
@@ -774,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -823,7 +811,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>10</v>
@@ -843,7 +831,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>10</v>
@@ -863,7 +851,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
@@ -883,7 +871,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>10</v>
@@ -897,13 +885,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>10</v>
@@ -923,7 +911,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>10</v>
@@ -943,7 +931,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>10</v>
@@ -957,13 +945,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>10</v>
@@ -983,7 +971,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>10</v>
@@ -1003,7 +991,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>10</v>
@@ -1023,7 +1011,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>10</v>
@@ -1043,7 +1031,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>10</v>
@@ -1063,7 +1051,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>10</v>
@@ -1083,7 +1071,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>10</v>
@@ -1103,7 +1091,7 @@
         <v>36</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>10</v>
@@ -1123,7 +1111,7 @@
         <v>38</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>10</v>
@@ -1143,7 +1131,7 @@
         <v>40</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>10</v>
@@ -1163,7 +1151,7 @@
         <v>42</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>10</v>
@@ -1183,7 +1171,7 @@
         <v>44</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>10</v>
@@ -1203,7 +1191,7 @@
         <v>46</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>10</v>
@@ -1223,7 +1211,7 @@
         <v>49</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>10</v>
@@ -1243,7 +1231,7 @@
         <v>50</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>10</v>
@@ -1263,7 +1251,7 @@
         <v>52</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>10</v>
@@ -1283,49 +1271,49 @@
         <v>54</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="5" t="s">
+    <row r="26" spans="1:6" ht="37.5" customHeight="1">
+      <c r="A26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1343,7 +1331,7 @@
         <v>60</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>10</v>
@@ -1363,49 +1351,49 @@
         <v>62</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="5" t="s">
+    <row r="30" spans="1:6" ht="45">
+      <c r="A30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="45">
-      <c r="A31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1423,49 +1411,9 @@
         <v>68</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F34" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Space removed Nov12 TC15 ECTEST
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CC5607-D517-41BD-931C-679ACA036F8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5E8808-EB01-4F16-AA59-EF63E86B5582}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,9 +138,6 @@
     <t>TC14_Verify_PlaceOrder_GuestUser</t>
   </si>
   <si>
-    <t>TC15_Verify _MyaccountSection_for_all_Usertype</t>
-  </si>
-  <si>
     <t>Verify Myaccounts Section for all type  of User</t>
   </si>
   <si>
@@ -250,6 +247,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>TC15_Verify_MyaccountSection_for_all_Usertype</t>
   </si>
 </sst>
 </file>
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -811,7 +811,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>10</v>
@@ -831,7 +831,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>10</v>
@@ -851,7 +851,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
@@ -871,7 +871,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>10</v>
@@ -885,13 +885,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>10</v>
@@ -911,7 +911,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>10</v>
@@ -931,7 +931,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>10</v>
@@ -945,13 +945,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>10</v>
@@ -971,7 +971,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>10</v>
@@ -991,7 +991,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>10</v>
@@ -1011,7 +1011,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>10</v>
@@ -1031,7 +1031,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>10</v>
@@ -1051,7 +1051,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>10</v>
@@ -1071,7 +1071,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>10</v>
@@ -1085,13 +1085,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="E16" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>10</v>
@@ -1105,13 +1105,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="E17" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>10</v>
@@ -1125,13 +1125,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="E18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>10</v>
@@ -1145,13 +1145,13 @@
         <v>7</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="E19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>10</v>
@@ -1165,13 +1165,13 @@
         <v>7</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="E20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>10</v>
@@ -1185,13 +1185,13 @@
         <v>7</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="E21" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>10</v>
@@ -1205,13 +1205,13 @@
         <v>7</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>10</v>
@@ -1225,13 +1225,13 @@
         <v>7</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>10</v>
@@ -1245,13 +1245,13 @@
         <v>7</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="E24" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>10</v>
@@ -1265,13 +1265,13 @@
         <v>7</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="E25" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>10</v>
@@ -1285,13 +1285,13 @@
         <v>7</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="E26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>10</v>
@@ -1305,13 +1305,13 @@
         <v>7</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="E27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>10</v>
@@ -1325,13 +1325,13 @@
         <v>7</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="E28" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>10</v>
@@ -1345,13 +1345,13 @@
         <v>7</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="E29" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>10</v>
@@ -1365,13 +1365,13 @@
         <v>7</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="E30" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>10</v>
@@ -1385,13 +1385,13 @@
         <v>7</v>
       </c>
       <c r="C31" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="E31" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>10</v>
@@ -1405,13 +1405,13 @@
         <v>7</v>
       </c>
       <c r="C32" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="E32" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
DOM Changes ECTEST - 18NOV
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5E8808-EB01-4F16-AA59-EF63E86B5582}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C94DB4-F797-4C9D-879E-82EFC807F6FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="70">
   <si>
     <t>Runmode</t>
   </si>
@@ -174,13 +174,7 @@
     <t>TC21_Verify_ Find_a_Branch_Guestuser</t>
   </si>
   <si>
-    <t>TC22_Verify_ Find_a_Branch_Loggedinuser</t>
-  </si>
-  <si>
     <t>Verify Find a Branch for GuestUser</t>
-  </si>
-  <si>
-    <t>Verify Find a Branch for loggedinUser</t>
   </si>
   <si>
     <t>TC23_Verify_Header</t>
@@ -387,7 +381,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -407,7 +401,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="8">
@@ -762,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -811,7 +804,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>10</v>
@@ -831,7 +824,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>10</v>
@@ -851,7 +844,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
@@ -871,7 +864,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>10</v>
@@ -885,13 +878,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>10</v>
@@ -911,7 +904,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>10</v>
@@ -931,7 +924,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>10</v>
@@ -945,13 +938,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>10</v>
@@ -971,7 +964,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>10</v>
@@ -991,7 +984,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>10</v>
@@ -1011,7 +1004,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>10</v>
@@ -1031,7 +1024,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>10</v>
@@ -1051,7 +1044,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>10</v>
@@ -1071,7 +1064,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>10</v>
@@ -1085,13 +1078,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>10</v>
@@ -1111,7 +1104,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>10</v>
@@ -1131,7 +1124,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>10</v>
@@ -1151,7 +1144,7 @@
         <v>41</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>10</v>
@@ -1171,7 +1164,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>10</v>
@@ -1191,7 +1184,7 @@
         <v>45</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>10</v>
@@ -1208,10 +1201,10 @@
         <v>46</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>10</v>
@@ -1224,14 +1217,14 @@
       <c r="B23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>47</v>
+      <c r="C23" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>10</v>
@@ -1251,49 +1244,49 @@
         <v>51</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="5" t="s">
+    <row r="25" spans="1:6" ht="37.5" customHeight="1">
+      <c r="A25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1311,7 +1304,7 @@
         <v>57</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>10</v>
@@ -1331,49 +1324,49 @@
         <v>59</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="5" t="s">
+    <row r="29" spans="1:6" ht="45">
+      <c r="A29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="45">
-      <c r="A30" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>62</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1384,36 +1377,16 @@
       <c r="B31" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>64</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TC23 Disabled for ECTEST
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C94DB4-F797-4C9D-879E-82EFC807F6FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E961019-F153-4540-BFAC-CCBA529C3A4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="68">
   <si>
     <t>Runmode</t>
   </si>
@@ -175,12 +175,6 @@
   </si>
   <si>
     <t>Verify Find a Branch for GuestUser</t>
-  </si>
-  <si>
-    <t>TC23_Verify_Header</t>
-  </si>
-  <si>
-    <t>Verify  all Header content</t>
   </si>
   <si>
     <t>TC24_Verify_PDP_Page</t>
@@ -755,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -804,7 +798,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>10</v>
@@ -824,7 +818,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>10</v>
@@ -844,7 +838,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
@@ -864,7 +858,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>10</v>
@@ -878,13 +872,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>10</v>
@@ -904,7 +898,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>10</v>
@@ -924,7 +918,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>10</v>
@@ -938,13 +932,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>10</v>
@@ -964,7 +958,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>10</v>
@@ -984,7 +978,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>10</v>
@@ -1004,7 +998,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>10</v>
@@ -1024,7 +1018,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>10</v>
@@ -1044,7 +1038,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>10</v>
@@ -1064,7 +1058,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>10</v>
@@ -1078,13 +1072,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>10</v>
@@ -1104,7 +1098,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>10</v>
@@ -1124,7 +1118,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>10</v>
@@ -1144,7 +1138,7 @@
         <v>41</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>10</v>
@@ -1164,7 +1158,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>10</v>
@@ -1184,7 +1178,7 @@
         <v>45</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>10</v>
@@ -1204,7 +1198,7 @@
         <v>47</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>10</v>
@@ -1224,49 +1218,49 @@
         <v>49</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="5" t="s">
+    <row r="24" spans="1:6" ht="37.5" customHeight="1">
+      <c r="A24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1284,7 +1278,7 @@
         <v>55</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>10</v>
@@ -1304,49 +1298,49 @@
         <v>57</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="5" t="s">
+    <row r="28" spans="1:6" ht="45">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="45">
-      <c r="A29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1364,29 +1358,9 @@
         <v>63</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Find a branch test case removal from PROD(TC19) and ECTEST(TC21)
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/MasterExecutor_Sanity.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\ECTEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vaibhav Oza\KAMAN_ECTEST_IE_SANITY-master\Input_files\Master_executors\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E961019-F153-4540-BFAC-CCBA529C3A4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="MasterExecutor" sheetId="10" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MasterExecutor!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MasterExecutor!$A$1:$F$29</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="66">
   <si>
     <t>Runmode</t>
   </si>
@@ -171,12 +170,6 @@
     <t>Type ahead must be displayed</t>
   </si>
   <si>
-    <t>TC21_Verify_ Find_a_Branch_Guestuser</t>
-  </si>
-  <si>
-    <t>Verify Find a Branch for GuestUser</t>
-  </si>
-  <si>
     <t>TC24_Verify_PDP_Page</t>
   </si>
   <si>
@@ -243,7 +236,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -399,13 +392,13 @@
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 2 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 5" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="4"/>
+    <cellStyle name="Normal 2 3" xfId="3"/>
+    <cellStyle name="Normal 2 4" xfId="6"/>
+    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="5"/>
+    <cellStyle name="Normal 5" xfId="7"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
@@ -748,11 +741,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -798,7 +791,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>10</v>
@@ -818,7 +811,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>10</v>
@@ -838,7 +831,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
@@ -858,7 +851,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>10</v>
@@ -872,13 +865,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>10</v>
@@ -898,7 +891,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>10</v>
@@ -918,7 +911,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>10</v>
@@ -932,13 +925,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>10</v>
@@ -958,7 +951,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>10</v>
@@ -978,7 +971,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>10</v>
@@ -998,7 +991,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>10</v>
@@ -1018,7 +1011,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>10</v>
@@ -1038,7 +1031,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>10</v>
@@ -1058,7 +1051,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>10</v>
@@ -1072,13 +1065,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>10</v>
@@ -1098,7 +1091,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>10</v>
@@ -1118,7 +1111,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>10</v>
@@ -1138,7 +1131,7 @@
         <v>41</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>10</v>
@@ -1158,7 +1151,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>10</v>
@@ -1178,7 +1171,7 @@
         <v>45</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>10</v>
@@ -1198,49 +1191,49 @@
         <v>47</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="5" t="s">
+    <row r="23" spans="1:6" ht="37.5" customHeight="1">
+      <c r="A23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1258,7 +1251,7 @@
         <v>53</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>10</v>
@@ -1278,49 +1271,49 @@
         <v>55</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="5" t="s">
+    <row r="27" spans="1:6" ht="45">
+      <c r="A27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="45">
-      <c r="A28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1338,33 +1331,14 @@
         <v>61</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:F29"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>